<commit_message>
zzf 费控 后台 2021-04-22 13:04:54
</commit_message>
<xml_diff>
--- a/PD/v5/assets/public/uploadCompany.xlsx
+++ b/PD/v5/assets/public/uploadCompany.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13433\Desktop\工作\物流费控\导入模板\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13433\Desktop\工作\物流费控\导入模板\新模板\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4D4ECD-4870-4EFB-8C8C-30A5A8A5B471}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7C163B-93F0-448E-873A-83834C1045D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="228" yWindow="768" windowWidth="22812" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="商家信息数据" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
+    <t>*商家ID</t>
+  </si>
+  <si>
     <t>*商家名称</t>
   </si>
   <si>
@@ -29,39 +32,13 @@
   </si>
   <si>
     <t>余额预警值</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>商家</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -87,30 +64,16 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -148,7 +111,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -469,31 +432,32 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="4" width="30" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25.05" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>